<commit_message>
update western data with new media ref
</commit_message>
<xml_diff>
--- a/PreparePipeline/western_summary.xlsx
+++ b/PreparePipeline/western_summary.xlsx
@@ -9,16 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12160" yWindow="1220" windowWidth="26960" windowHeight="14500" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="12160" yWindow="1220" windowWidth="26960" windowHeight="14500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="110917" sheetId="2" r:id="rId1"/>
+    <sheet name="Western_summary.csv" sheetId="3" r:id="rId2"/>
+    <sheet name="Table" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$R$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'110917'!$A$1:$R$1</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="39">
   <si>
     <t>#</t>
   </si>
@@ -77,9 +76,6 @@
     <t>BCS_MEDIA</t>
   </si>
   <si>
-    <t>ALT</t>
-  </si>
-  <si>
     <t>L. crispatus</t>
   </si>
   <si>
@@ -129,6 +125,30 @@
   </si>
   <si>
     <t>Ljen</t>
+  </si>
+  <si>
+    <t>052917, run 061517, pg 26 miRNA5 NB</t>
+  </si>
+  <si>
+    <t>110917</t>
+  </si>
+  <si>
+    <t>101417</t>
+  </si>
+  <si>
+    <t>052917, run 081217, pg 45 miRNA5 NB</t>
+  </si>
+  <si>
+    <t>ALT (normalized to media within blot on run day)</t>
+  </si>
+  <si>
+    <t>022617</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Non_media_ref</t>
   </si>
 </sst>
 </file>
@@ -138,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,17 +180,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
     </font>
     <font>
       <i/>
@@ -225,10 +234,10 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -243,7 +252,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -252,8 +261,6 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -263,6 +270,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -543,198 +551,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A50"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="12"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="12"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="12"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="12"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="12"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="12"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="12"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="12"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="12"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="12"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="12"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="12"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="12"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="12"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="12"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="12"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="12"/>
-    </row>
-  </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A3:A4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2128,12 +1944,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2141,10 +1957,10 @@
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="41" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2158,12 +1974,18 @@
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -2172,15 +1994,19 @@
         <v>2.5749200000000001E-4</v>
       </c>
       <c r="D2" s="1">
+        <f>C2/$C$7</f>
+        <v>6.6867032460732993E-3</v>
+      </c>
+      <c r="E2" s="1">
         <v>2.4E-2</v>
       </c>
-      <c r="E2" s="1">
-        <v>6.6867032460732993E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -2189,13 +2015,16 @@
         <v>1.1103151862464184E-3</v>
       </c>
       <c r="D3" s="1">
+        <f t="shared" ref="D3:D7" si="0">C3/$C$7</f>
         <v>2.8833315831320604E-2</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -2204,12 +2033,16 @@
         <v>7.8388278388278384E-3</v>
       </c>
       <c r="D4" s="1">
+        <f t="shared" si="0"/>
         <v>0.20356327790882764</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -2218,12 +2051,16 @@
         <v>1.5801011804384486E-2</v>
       </c>
       <c r="D5" s="1">
+        <f>C5/$C$7</f>
         <v>0.41032994005103174</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -2232,12 +2069,16 @@
         <v>4.6985446985446985E-3</v>
       </c>
       <c r="D6" s="1">
+        <f t="shared" si="0"/>
         <v>0.12201456389938066</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -2246,56 +2087,88 @@
         <v>3.850806451612903E-2</v>
       </c>
       <c r="D7" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>13</v>
       </c>
+      <c r="C8">
+        <v>6.320422535211267E-4</v>
+      </c>
       <c r="D8" s="1">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <f>C8/$C$13</f>
+        <v>0.1516901408450704</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>13</v>
       </c>
+      <c r="C9">
+        <v>1.0488505747126436E-3</v>
+      </c>
       <c r="D9" s="1">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="D9:D13" si="1">C9/$C$13</f>
+        <v>0.25172413793103449</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>13</v>
       </c>
+      <c r="C10">
+        <v>5.5677154582763344E-3</v>
+      </c>
       <c r="D10" s="1">
-        <v>1.34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>1.3362517099863203</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>13</v>
       </c>
+      <c r="C11">
+        <v>4.5012165450121653E-3</v>
+      </c>
       <c r="D11" s="1">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>1.0802919708029197</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>13</v>
@@ -2304,23 +2177,37 @@
         <v>2.8195490000000002E-3</v>
       </c>
       <c r="D12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.67669176000000009</v>
+      </c>
+      <c r="E12" s="1">
         <v>0.43120000000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F12" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>13</v>
       </c>
+      <c r="C13">
+        <v>4.1666666666666666E-3</v>
+      </c>
       <c r="D13" s="1">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>22</v>
@@ -2329,15 +2216,19 @@
         <v>3.58115E-4</v>
       </c>
       <c r="D14" s="1">
+        <f>C14/$C$19</f>
+        <v>4.4764374999999995E-2</v>
+      </c>
+      <c r="E14" s="1">
         <v>5.4769999999999999E-2</v>
       </c>
-      <c r="E14" s="1">
-        <v>4.4764374999999995E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F14" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>22</v>
@@ -2346,12 +2237,16 @@
         <v>1.9189944134078213E-3</v>
       </c>
       <c r="D15" s="1">
+        <f t="shared" ref="D15:D19" si="2">C15/$C$19</f>
         <v>0.23987430167597765</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>22</v>
@@ -2360,12 +2255,16 @@
         <v>1.2287735849056604E-2</v>
       </c>
       <c r="D16" s="1">
+        <f t="shared" si="2"/>
         <v>1.5359669811320755</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F16" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>22</v>
@@ -2374,12 +2273,16 @@
         <v>2.1157684630738523E-2</v>
       </c>
       <c r="D17" s="1">
+        <f t="shared" si="2"/>
         <v>2.6447105788423153</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F17" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>22</v>
@@ -2388,12 +2291,16 @@
         <v>7.1307300509337859E-3</v>
       </c>
       <c r="D18" s="1">
+        <f t="shared" si="2"/>
         <v>0.89134125636672323</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F18" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>22</v>
@@ -2402,12 +2309,16 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D19" s="1">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F19" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>24</v>
@@ -2419,10 +2330,17 @@
         <f>C20/$C$19</f>
         <v>4.7189922480620154</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20">
+        <f>C20/C21</f>
+        <v>0.52103158961653251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21">
         <v>24</v>
@@ -2431,13 +2349,16 @@
         <v>7.2456140350877191E-2</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" ref="D21:D26" si="0">C21/$C$19</f>
+        <f t="shared" ref="D21:D26" si="3">C21/$C$19</f>
         <v>9.057017543859649</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F21" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>24</v>
@@ -2446,13 +2367,16 @@
         <v>5.5507088331515811E-2</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6.9383860414394762</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F22" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <v>24</v>
@@ -2461,13 +2385,16 @@
         <v>6.1111111111111109E-2</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7.6388888888888884</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F23" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24">
         <v>24</v>
@@ -2476,13 +2403,16 @@
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5.5555555555555554</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F24" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -2491,13 +2421,16 @@
         <v>0.11392405063291139</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>14.240506329113924</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F25" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26">
         <v>24</v>
@@ -2506,8 +2439,11 @@
         <v>2.4538545059717701E-2</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.0673181324647127</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2519,7 +2455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -2536,30 +2472,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
+      <c r="A2" s="13"/>
       <c r="B2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6">
         <v>2.4E-2</v>
@@ -2573,7 +2509,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="6">
         <v>2.8833315831320604E-2</v>
@@ -2587,7 +2523,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="6">
         <v>0.20356327790882764</v>
@@ -2601,7 +2537,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6">
         <v>0.41032994005103174</v>
@@ -2615,7 +2551,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="6">
         <v>0.12201456389938066</v>
@@ -2629,7 +2565,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>

</xml_diff>